<commit_message>
Update to test phase
</commit_message>
<xml_diff>
--- a/src/main/resources/static/Team Information.xlsx
+++ b/src/main/resources/static/Team Information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akin Akinbobola\IdeaProjects\dailybot\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E3DF22-DC17-42BA-BA42-6242E45801F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88338A94-E79B-49D8-8074-889BFE5F7309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:Z60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>